<commit_message>
fix formula of the expectation value
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -5,23 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/Lemmings/Assets/Script/AI/config_gen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3017A2-21E2-624C-86E3-F28472FC5538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B3FC9-D06E-B647-A770-1E26EC8490BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
     <sheet name="actors" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="185">
   <si>
     <t>ID</t>
   </si>
@@ -94,79 +107,52 @@
     <t>Strong</t>
   </si>
   <si>
-    <t>HP:2</t>
-  </si>
-  <si>
     <t>LD1-B1</t>
   </si>
   <si>
     <t>MP</t>
   </si>
   <si>
-    <t>MP:2</t>
-  </si>
-  <si>
     <t>LD1-C1</t>
   </si>
   <si>
     <t>Gold</t>
   </si>
   <si>
-    <t>Gold:2</t>
-  </si>
-  <si>
     <t>LD2-A1</t>
   </si>
   <si>
     <t>Ability1</t>
   </si>
   <si>
-    <t>Ability1:2</t>
-  </si>
-  <si>
     <t>LD2-B1</t>
   </si>
   <si>
     <t>Ability2</t>
   </si>
   <si>
-    <t>Ability2:2</t>
-  </si>
-  <si>
     <t>LD2-C1</t>
   </si>
   <si>
     <t>Ability3</t>
   </si>
   <si>
-    <t>Ability3:2</t>
-  </si>
-  <si>
     <t>LD3-A1</t>
   </si>
   <si>
     <t>Resource1</t>
   </si>
   <si>
-    <t>Resource1:2</t>
-  </si>
-  <si>
     <t>LD3-B1</t>
   </si>
   <si>
     <t>Resource2</t>
   </si>
   <si>
-    <t>Resource2:2</t>
-  </si>
-  <si>
     <t>LD3-C1</t>
   </si>
   <si>
     <t>Resource3</t>
-  </si>
-  <si>
-    <t>Resource3:2</t>
   </si>
   <si>
     <t>LD0-1</t>
@@ -432,9 +418,6 @@
   </si>
   <si>
     <t>SM_Env_GrassPath_Corner_03</t>
-  </si>
-  <si>
-    <t>SM_Env_GrassPath_Straight_04</t>
   </si>
   <si>
     <t>isFly</t>
@@ -452,9 +435,6 @@
 핫도그는 살안쪄요~</t>
   </si>
   <si>
-    <t>HP Script</t>
-  </si>
-  <si>
     <t>MP Script</t>
   </si>
   <si>
@@ -504,6 +484,151 @@
   <si>
     <t>satisfactions
 Refusal</t>
+  </si>
+  <si>
+    <t>ACTOR1-3</t>
+  </si>
+  <si>
+    <t>ACTOR1-4</t>
+  </si>
+  <si>
+    <t>ACTOR1-5</t>
+  </si>
+  <si>
+    <t>ACTOR1-6</t>
+  </si>
+  <si>
+    <t>ACTOR1-7</t>
+  </si>
+  <si>
+    <t>ACTOR1-8</t>
+  </si>
+  <si>
+    <t>ACTOR1-9</t>
+  </si>
+  <si>
+    <t>Actors/actor3</t>
+  </si>
+  <si>
+    <t>Actors/actor4</t>
+  </si>
+  <si>
+    <t>Actors/actor6</t>
+  </si>
+  <si>
+    <t>Actors/actor9</t>
+  </si>
+  <si>
+    <t>포그니</t>
+  </si>
+  <si>
+    <t>김밥이</t>
+  </si>
+  <si>
+    <t>인절미</t>
+  </si>
+  <si>
+    <t>성실이</t>
+  </si>
+  <si>
+    <t>쭈녕이</t>
+  </si>
+  <si>
+    <t>고기봉</t>
+  </si>
+  <si>
+    <t>캬옹이</t>
+  </si>
+  <si>
+    <t>HP,27,50,30
+MP,20,50,21
+Gold,20,50,10
+Ability1,20,50,10
+Ability2,20,50,10
+Ability3,20,50,10
+Resource1,20,50,10
+Resource2,20,50,10
+Resource3,20,50,10
+Sight,20,50,10
+Leadership,0,50,10
+Friendship,0,50,10</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>HP:4</t>
+  </si>
+  <si>
+    <t>MP:4</t>
+  </si>
+  <si>
+    <t>Gold:4</t>
+  </si>
+  <si>
+    <t>Ability1:4,HP:-2</t>
+  </si>
+  <si>
+    <t>Ability2:4,MP:-2</t>
+  </si>
+  <si>
+    <t>Ability3:4,HP:-1,MP-1</t>
+  </si>
+  <si>
+    <t>Resource1:4,Ability1:-2</t>
+  </si>
+  <si>
+    <t>Resource2:4,Ability2:-2</t>
+  </si>
+  <si>
+    <t>Resource3:4,Ability3:-2</t>
+  </si>
+  <si>
+    <t>체력이 올라간다~</t>
+  </si>
+  <si>
+    <t>Actors/npc7</t>
+  </si>
+  <si>
+    <t>Actors/npc5</t>
+  </si>
+  <si>
+    <t>Actors/npc8</t>
+  </si>
+  <si>
+    <t>NPC-104</t>
+  </si>
+  <si>
+    <t>맥주 팔기</t>
+  </si>
+  <si>
+    <t>맥주 팝니다~</t>
+  </si>
+  <si>
+    <t>1,100</t>
+  </si>
+  <si>
+    <t>HP,15,90,85
+MP,0,100,10
+Gold,10,20,100</t>
   </si>
 </sst>
 </file>
@@ -1363,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1381,6 +1506,7 @@
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" style="4"/>
     <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
@@ -1401,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1416,7 +1542,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1434,33 +1560,36 @@
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="R1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="S1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="I2" s="1">
         <v>2</v>
@@ -1471,70 +1600,67 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1">
         <v>0</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="Q2" s="4">
         <v>102</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
+        <v>180</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
       </c>
       <c r="J3">
         <v>-1</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1"/>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="Q3" s="4">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1546,10 +1672,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -1563,25 +1686,25 @@
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
-        <v>120</v>
+      <c r="L4" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="Q4" s="4">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1593,7 +1716,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -1607,25 +1733,25 @@
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>121</v>
+      <c r="L5" t="s">
+        <v>111</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="Q5" s="4">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1637,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -1652,24 +1778,24 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="Q6" s="4">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1681,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
         <v>17</v>
@@ -1696,24 +1822,24 @@
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="Q7" s="4">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1725,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -1740,24 +1866,24 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="Q8" s="4">
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1769,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -1784,24 +1910,24 @@
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>36</v>
+        <v>172</v>
       </c>
       <c r="Q9" s="4">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1813,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H10" t="s">
         <v>17</v>
@@ -1828,24 +1954,24 @@
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>39</v>
+        <v>173</v>
       </c>
       <c r="Q10" s="4">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1857,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
         <v>17</v>
@@ -1872,27 +1998,24 @@
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="Q11" s="4">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1904,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -1919,27 +2042,30 @@
         <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>46</v>
+        <v>175</v>
       </c>
       <c r="Q12" s="4">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1948,7 +2074,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -1963,24 +2089,27 @@
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
+      <c r="O13" t="s">
+        <v>37</v>
+      </c>
       <c r="Q13" s="4">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -1989,45 +2118,39 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K14">
-        <v>3</v>
-      </c>
-      <c r="L14" t="s">
-        <v>107</v>
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>51</v>
-      </c>
-      <c r="O14" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="4">
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
@@ -2036,34 +2159,81 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
         <v>-1</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>4</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
-        <v>147</v>
-      </c>
-      <c r="S15" t="s">
-        <v>148</v>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>136</v>
+      </c>
+      <c r="S16" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2073,10 +2243,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2095,54 +2265,54 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" t="s">
-        <v>66</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="P1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2154,25 +2324,25 @@
         <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
@@ -2180,7 +2350,7 @@
     </row>
     <row r="3" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -2192,19 +2362,19 @@
         <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -2213,7 +2383,7 @@
         <v>15</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="P3" t="b">
         <v>0</v>
@@ -2221,7 +2391,7 @@
     </row>
     <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -2233,19 +2403,19 @@
         <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>178</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -2254,15 +2424,15 @@
         <v>15</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -2274,25 +2444,25 @@
         <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>78</v>
+        <v>184</v>
       </c>
       <c r="P5" t="b">
         <v>0</v>
@@ -2300,7 +2470,7 @@
     </row>
     <row r="6" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2312,19 +2482,19 @@
         <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -2333,7 +2503,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P6" t="b">
         <v>0</v>
@@ -2341,7 +2511,7 @@
     </row>
     <row r="7" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -2353,19 +2523,19 @@
         <v>106</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -2374,7 +2544,7 @@
         <v>20</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P7" t="b">
         <v>0</v>
@@ -2382,7 +2552,7 @@
     </row>
     <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -2394,25 +2564,25 @@
         <v>107</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P8" t="b">
         <v>1</v>
@@ -2420,7 +2590,7 @@
     </row>
     <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -2432,39 +2602,39 @@
         <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -2473,39 +2643,39 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="P10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -2514,27 +2684,314 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="P11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>154</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>155</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>150</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="204" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2542,4 +2999,151 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511382C-D11B-5A44-B5FF-0A23CC8CA529}">
+  <dimension ref="K1:U11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>32</v>
+      </c>
+      <c r="N2">
+        <v>50</v>
+      </c>
+      <c r="O2">
+        <f>(M2-L2) / (N2-L2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="P2">
+        <f>IF(O2 &lt; 0, O2*2, O2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q2">
+        <f>POWER(P2-O5,2)</f>
+        <v>0.23901234567901233</v>
+      </c>
+    </row>
+    <row r="3" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O4" si="0">(M3-L3) / (N3-L3)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P4" si="1">IF(O3 &lt; 0, O3*2, O3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>POWER(P3-O5,2)</f>
+        <v>7.9012345679012295E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>50</v>
+      </c>
+      <c r="O4">
+        <f>((M4-L4) / (N4-L4))</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="Q4">
+        <f>POWER(P4-O5,2)</f>
+        <v>0.3338271604938271</v>
+      </c>
+    </row>
+    <row r="5" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>160</v>
+      </c>
+      <c r="O5">
+        <f>(P2+P3+P4) / 3</f>
+        <v>-8.8888888888888865E-2</v>
+      </c>
+      <c r="Q5">
+        <f>SQRT((Q2+Q3+Q4) /3)</f>
+        <v>0.4399775527382962</v>
+      </c>
+    </row>
+    <row r="7" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>166</v>
+      </c>
+      <c r="O7">
+        <f>O5/Q5</f>
+        <v>-0.20203050891044211</v>
+      </c>
+    </row>
+    <row r="9" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="U9">
+        <v>-0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <v>-0.17191799999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="11:21" x14ac:dyDescent="0.2">
+      <c r="U11">
+        <v>-0.1867</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix that satisfaction value never over the max
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B3FC9-D06E-B647-A770-1E26EC8490BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C919DA6-203F-7549-A3EF-F1373AF36D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -433,12 +433,6 @@
 핫도그 맛있어요~
 웰빙 핫도그 드셔보세요~
 핫도그는 살안쪄요~</t>
-  </si>
-  <si>
-    <t>MP Script</t>
-  </si>
-  <si>
-    <t>Gold Script</t>
   </si>
   <si>
     <t>Ability1 Script</t>
@@ -623,12 +617,16 @@
     <t>맥주 팝니다~</t>
   </si>
   <si>
-    <t>1,100</t>
-  </si>
-  <si>
     <t>HP,15,90,85
 MP,0,100,10
 Gold,10,20,100</t>
+  </si>
+  <si>
+    <t>정신력이 올라간다~</t>
+  </si>
+  <si>
+    <t>돈이 왠수지
+돈벌기는 왜 항상 힘들지</t>
   </si>
 </sst>
 </file>
@@ -1490,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1542,7 +1540,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1560,7 +1558,7 @@
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>13</v>
@@ -1572,15 +1570,15 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>183</v>
+      <c r="D2" t="s">
+        <v>15</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1617,19 +1615,19 @@
     </row>
     <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>183</v>
+      <c r="D3" t="s">
+        <v>15</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H3" t="s">
         <v>101</v>
@@ -1655,7 +1653,7 @@
         <v>104</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1681,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1693,13 +1691,13 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q4" s="4">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1728,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1740,13 +1738,13 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q5" s="4">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="51" x14ac:dyDescent="0.2">
@@ -1784,13 +1782,13 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q6" s="4">
         <v>1</v>
       </c>
-      <c r="R6" t="s">
-        <v>126</v>
+      <c r="R6" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1828,13 +1826,13 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q7" s="4">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1872,13 +1870,13 @@
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="Q8" s="4">
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1916,13 +1914,13 @@
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q9" s="4">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="34" x14ac:dyDescent="0.2">
@@ -1960,13 +1958,13 @@
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q10" s="4">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -2004,13 +2002,13 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q11" s="4">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -2048,13 +2046,13 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q12" s="4">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -2101,7 +2099,7 @@
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -2142,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -2189,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -2230,10 +2228,10 @@
         <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="S16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2245,7 +2243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -2368,7 +2366,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>62</v>
@@ -2409,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>68</v>
@@ -2450,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>73</v>
@@ -2462,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P5" t="b">
         <v>0</v>
@@ -2661,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P10" t="b">
         <v>0</v>
@@ -2702,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P11" t="b">
         <v>0</v>
@@ -2710,7 +2708,7 @@
     </row>
     <row r="12" spans="1:16" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -2725,13 +2723,13 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>106</v>
@@ -2743,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P12" t="b">
         <v>0</v>
@@ -2751,7 +2749,7 @@
     </row>
     <row r="13" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -2766,13 +2764,13 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>106</v>
@@ -2784,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P13" t="b">
         <v>0</v>
@@ -2792,7 +2790,7 @@
     </row>
     <row r="14" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -2807,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2825,7 +2823,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -2833,7 +2831,7 @@
     </row>
     <row r="15" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -2848,13 +2846,13 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>106</v>
@@ -2866,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P15" t="b">
         <v>0</v>
@@ -2874,7 +2872,7 @@
     </row>
     <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -2889,7 +2887,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2907,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P16" t="b">
         <v>0</v>
@@ -2915,7 +2913,7 @@
     </row>
     <row r="17" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -2930,7 +2928,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2948,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P17" t="b">
         <v>0</v>
@@ -2956,7 +2954,7 @@
     </row>
     <row r="18" spans="1:16" ht="204" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -2971,13 +2969,13 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>106</v>
@@ -2989,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P18" t="b">
         <v>0</v>
@@ -3013,19 +3011,19 @@
   <sheetData>
     <row r="1" spans="11:21" x14ac:dyDescent="0.2">
       <c r="L1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N1" t="s">
         <v>162</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" t="s">
         <v>163</v>
-      </c>
-      <c r="N1" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="11:21" x14ac:dyDescent="0.2">
@@ -3068,7 +3066,7 @@
         <v>50</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O4" si="0">(M3-L3) / (N3-L3)</f>
+        <f t="shared" ref="O3" si="0">(M3-L3) / (N3-L3)</f>
         <v>0</v>
       </c>
       <c r="P3">
@@ -3108,7 +3106,7 @@
     </row>
     <row r="5" spans="11:21" x14ac:dyDescent="0.2">
       <c r="N5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O5">
         <f>(P2+P3+P4) / 3</f>
@@ -3121,7 +3119,7 @@
     </row>
     <row r="7" spans="11:21" x14ac:dyDescent="0.2">
       <c r="N7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="O7">
         <f>O5/Q5</f>

</xml_diff>

<commit_message>
fix for task UI
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE83816-25D4-6D42-BE26-42B9600A54FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2733308D-B29C-A143-94FF-FB1EE07FBB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="326">
   <si>
     <t>ID</t>
   </si>
@@ -125,48 +125,27 @@
     <t>LD2-A1</t>
   </si>
   <si>
-    <t>Ability1</t>
-  </si>
-  <si>
     <t>LD2-B1</t>
   </si>
   <si>
-    <t>Ability2</t>
-  </si>
-  <si>
     <t>LD2-C1</t>
   </si>
   <si>
-    <t>Ability3</t>
-  </si>
-  <si>
     <t>LD3-A1</t>
   </si>
   <si>
-    <t>Resource1</t>
-  </si>
-  <si>
     <t>LD3-B1</t>
   </si>
   <si>
-    <t>Resource2</t>
-  </si>
-  <si>
     <t>LD3-C1</t>
   </si>
   <si>
-    <t>Resource3</t>
-  </si>
-  <si>
     <t>LD0-1</t>
   </si>
   <si>
     <t>LD0-1-C</t>
   </si>
   <si>
-    <t>Sight1</t>
-  </si>
-  <si>
     <t>Sight:2</t>
   </si>
   <si>
@@ -176,9 +155,6 @@
     <t>LD4-1</t>
   </si>
   <si>
-    <t>Leadership1</t>
-  </si>
-  <si>
     <t>Greeting</t>
   </si>
   <si>
@@ -186,9 +162,6 @@
   </si>
   <si>
     <t>Leadership:2</t>
-  </si>
-  <si>
-    <t>Leadership1 Interaction</t>
   </si>
   <si>
     <t>Friendship:1</t>
@@ -347,9 +320,6 @@
   </si>
   <si>
     <t>PET1-1</t>
-  </si>
-  <si>
-    <t>무당한테 점보기</t>
   </si>
   <si>
     <t>1.Satisfaction.gold:max</t>
@@ -572,33 +542,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>HP:4</t>
-  </si>
-  <si>
-    <t>MP:4</t>
-  </si>
-  <si>
-    <t>Gold:4</t>
-  </si>
-  <si>
-    <t>Ability1:4,HP:-2</t>
-  </si>
-  <si>
-    <t>Ability2:4,MP:-2</t>
-  </si>
-  <si>
-    <t>Ability3:4,HP:-1,MP-1</t>
-  </si>
-  <si>
-    <t>Resource1:4,Ability1:-2</t>
-  </si>
-  <si>
-    <t>Resource2:4,Ability2:-2</t>
-  </si>
-  <si>
-    <t>Resource3:4,Ability3:-2</t>
-  </si>
-  <si>
     <t>체력이 올라간다~</t>
   </si>
   <si>
@@ -903,18 +846,6 @@
     <t>lv.10</t>
   </si>
   <si>
-    <t>TaskCounter,10</t>
-  </si>
-  <si>
-    <t>TaskCounter,20</t>
-  </si>
-  <si>
-    <t>TaskCounter,40</t>
-  </si>
-  <si>
-    <t>TaskCounter,80</t>
-  </si>
-  <si>
     <t>TaskCounter,100</t>
   </si>
   <si>
@@ -1016,52 +947,227 @@
 2</t>
   </si>
   <si>
-    <t>&lt;size=100%&gt;체력 올리기&lt;/size&gt;
-&lt;size=80%&gt;체력을 올린다 &lt;color=#E4CA44&gt;체력 +4&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;점쟁이에게 내가 여기 왜 왔는지 물어보기&lt;/size&gt;
-&lt;size=80%&gt;점쟁이로 부터 정신적 안정감을 얻는다 &lt;color=#E4CA44&gt;정신력 +4&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;돈벌기&lt;/size&gt;
-&lt;size=80%&gt;골드를 벌기위해 일한다  &lt;color=#E4CA44&gt;골드 +4&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;Ability1&lt;/size&gt;
-&lt;size=80%&gt;Ability1을 올린다 &lt;color=#E4CA44&gt;체력 -2&lt;/color&gt;, &lt;color=#428644&gt;Ability1 +4&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;Ability2&lt;/size&gt;
-&lt;size=80%&gt;Ability2을 올린다 &lt;color=#E4CA44&gt;정신력 -2&lt;/color&gt;, &lt;color=#428644&gt;Ability2 +4&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;Ability3&lt;/size&gt;
-&lt;size=80%&gt;Ability3을 올린다 &lt;color=#E4CA44&gt;체력 -1, 정신력 -1&lt;/color&gt;, &lt;color=#428644&gt;Ability3 +4&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;Resource1&lt;/size&gt;
-&lt;size=80%&gt;Resource1 구하기 &lt;color=#E4CA44&gt;Ability1 -2&lt;/color&gt;, &lt;color=#428644&gt;Resource1 +4&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;Resource2&lt;/size&gt;
-&lt;size=80%&gt;Resource2 구하기 &lt;color=#E4CA44&gt;Ability2 -2&lt;/color&gt;, &lt;color=#428644&gt;Resource2 +4&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;Resource3&lt;/size&gt;
-&lt;size=80%&gt;Resource3 구하기 &lt;color=#E4CA44&gt;Ability3 -2&lt;/color&gt;, &lt;color=#428644&gt;Resource3 +4&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;시야 넓히기&lt;/size&gt;
-&lt;size=80%&gt;다른 마을을 보고 온다 &lt;color=#428644&gt;시야 +2&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;리더십키우기&lt;/size&gt;
-&lt;size=80%&gt;주변에 돈많을 사람한테 괜히 말걸기  &lt;color=#428644&gt;리더십 +2&lt;/color&gt; &lt;/size&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=100%&gt;괜히 말을 걸어왔습니다.&lt;/size&gt;
-&lt;size=80%&gt;받아주면 &lt;color=#E4CA44&gt;친근감 +1&lt;/color&gt;&lt;/size&gt;</t>
+    <t>체력 올리기</t>
+  </si>
+  <si>
+    <t>체력을 올린다</t>
+  </si>
+  <si>
+    <t>점쟁이에게 내가 여기 왜 왔는지 물어보기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">점쟁이로 부터 정신적 안정감을 얻는다 </t>
+  </si>
+  <si>
+    <t>돈벌기</t>
+  </si>
+  <si>
+    <t>골드를 벌기위해 일한다</t>
+  </si>
+  <si>
+    <t>생산력1</t>
+  </si>
+  <si>
+    <t>생산력2</t>
+  </si>
+  <si>
+    <t>생산력3</t>
+  </si>
+  <si>
+    <t>자원1</t>
+  </si>
+  <si>
+    <t>자원2</t>
+  </si>
+  <si>
+    <t>자원3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">생산력1을 올린다 </t>
+  </si>
+  <si>
+    <t>자원1 구하기</t>
+  </si>
+  <si>
+    <t>시야 넓히기</t>
+  </si>
+  <si>
+    <t>다른 마을을 보고 온다</t>
+  </si>
+  <si>
+    <t>리더십키우기</t>
+  </si>
+  <si>
+    <t>주변에 돈많을 사람한테 괜히 말걸기</t>
+  </si>
+  <si>
+    <t>괜히 말을 걸어왔습니다</t>
+  </si>
+  <si>
+    <t>받아주면</t>
+  </si>
+  <si>
+    <t>HP:4,Gold:-2</t>
+  </si>
+  <si>
+    <t>MP:4,HP:-2</t>
+  </si>
+  <si>
+    <t>Gold:4,MP:-2</t>
+  </si>
+  <si>
+    <t>Ability1:4,HP:-4</t>
+  </si>
+  <si>
+    <t>Ability2:4,MP:-4</t>
+  </si>
+  <si>
+    <t>Ability3:4,HP:-2,MP:-2</t>
+  </si>
+  <si>
+    <t>Resource1:4,Ability1:-6</t>
+  </si>
+  <si>
+    <t>Resource2:4,Ability2:-6</t>
+  </si>
+  <si>
+    <t>Resource3:4,Ability3:-6</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,0</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,1</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,2</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,3</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,4</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,5</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,6</t>
+  </si>
+  <si>
+    <t>HP,27,50,8
+MP,20,50,8
+Gold,20,50,8
+Ability1,20,50,0
+Ability2,20,50,0
+Ability3,20,50,0
+Resource1,20,50,0
+Resource2,20,50,0
+Resource3,20,50,0
+Sight,20,50,0
+Leadership,0,50,0
+Friendship,0,50,7</t>
+  </si>
+  <si>
+    <t>4,10</t>
+  </si>
+  <si>
+    <t>5,10</t>
+  </si>
+  <si>
+    <t>2,10</t>
+  </si>
+  <si>
+    <t>3,10</t>
+  </si>
+  <si>
+    <t>TaskCounter,16</t>
+  </si>
+  <si>
+    <t>TaskCounter,8</t>
+  </si>
+  <si>
+    <t>TaskCounter,32</t>
+  </si>
+  <si>
+    <t>TaskCounter,64</t>
   </si>
 </sst>
 </file>
@@ -1935,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1951,7 +2057,7 @@
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" customWidth="1"/>
-    <col min="15" max="15" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" style="4"/>
     <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
@@ -1972,7 +2078,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1987,7 +2093,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -2005,21 +2111,21 @@
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="R1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="S1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -2031,10 +2137,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I2" s="1">
         <v>2</v>
@@ -2051,18 +2157,18 @@
       </c>
       <c r="N2" s="1"/>
       <c r="O2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q2" s="4">
         <v>102</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -2074,10 +2180,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I3" s="1">
         <v>2</v>
@@ -2094,16 +2200,16 @@
       </c>
       <c r="N3" s="1"/>
       <c r="O3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q3" s="4">
         <v>104</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2117,10 +2223,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>281</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -2129,28 +2235,28 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>165</v>
+        <v>301</v>
       </c>
       <c r="Q4" s="4">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2164,10 +2270,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>283</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -2176,25 +2282,25 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>166</v>
+        <v>302</v>
       </c>
       <c r="Q5" s="4">
         <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="51" x14ac:dyDescent="0.2">
@@ -2211,10 +2317,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>285</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -2229,22 +2335,22 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>167</v>
+        <v>303</v>
       </c>
       <c r="Q6" s="4">
         <v>1</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2252,16 +2358,16 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>320</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>287</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="H7" t="s">
         <v>17</v>
@@ -2276,39 +2382,39 @@
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>168</v>
+        <v>304</v>
       </c>
       <c r="Q7" s="4">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>320</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>288</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -2323,39 +2429,39 @@
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="Q8" s="4">
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>320</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>289</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -2370,39 +2476,39 @@
         <v>1</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="O9" t="s">
-        <v>170</v>
+        <v>306</v>
       </c>
       <c r="Q9" s="4">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>321</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>290</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="H10" t="s">
         <v>17</v>
@@ -2417,39 +2523,39 @@
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="O10" t="s">
-        <v>171</v>
+        <v>307</v>
       </c>
       <c r="Q10" s="4">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>321</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>291</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="H11" t="s">
         <v>17</v>
@@ -2464,39 +2570,39 @@
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>172</v>
+        <v>308</v>
       </c>
       <c r="Q11" s="4">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>321</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>292</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -2511,42 +2617,42 @@
         <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>173</v>
+        <v>309</v>
       </c>
       <c r="Q12" s="4">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>318</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>295</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -2561,36 +2667,36 @@
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="4">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>318</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
@@ -2606,7 +2712,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2615,30 +2721,30 @@
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>319</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>297</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2650,27 +2756,27 @@
         <v>3</v>
       </c>
       <c r="L15" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="O15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="Q15" s="4">
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2682,13 +2788,13 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>299</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -2703,19 +2809,20 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="Q16" s="4">
         <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="S16" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2724,8 +2831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2744,54 +2851,54 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>57</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="P1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2803,25 +2910,25 @@
         <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
@@ -2829,7 +2936,7 @@
     </row>
     <row r="3" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -2841,19 +2948,19 @@
         <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -2862,7 +2969,7 @@
         <v>15</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="P3" t="b">
         <v>0</v>
@@ -2870,7 +2977,7 @@
     </row>
     <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -2882,19 +2989,19 @@
         <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -2903,7 +3010,7 @@
         <v>15</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P4" t="b">
         <v>0</v>
@@ -2911,7 +3018,7 @@
     </row>
     <row r="5" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -2923,25 +3030,25 @@
         <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="P5" t="b">
         <v>0</v>
@@ -2949,7 +3056,7 @@
     </row>
     <row r="6" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2961,19 +3068,19 @@
         <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -2982,7 +3089,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P6" t="b">
         <v>0</v>
@@ -2990,7 +3097,7 @@
     </row>
     <row r="7" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -3002,19 +3109,19 @@
         <v>106</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -3023,7 +3130,7 @@
         <v>20</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P7" t="b">
         <v>0</v>
@@ -3031,7 +3138,7 @@
     </row>
     <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -3043,25 +3150,25 @@
         <v>107</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P8" t="b">
         <v>1</v>
@@ -3069,7 +3176,7 @@
     </row>
     <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3081,25 +3188,25 @@
         <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P9" t="b">
         <v>0</v>
@@ -3107,13 +3214,13 @@
     </row>
     <row r="10" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -3122,25 +3229,25 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>157</v>
+        <v>310</v>
       </c>
       <c r="P10" t="b">
         <v>0</v>
@@ -3148,13 +3255,13 @@
     </row>
     <row r="11" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -3163,25 +3270,25 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>157</v>
+        <v>311</v>
       </c>
       <c r="P11" t="b">
         <v>0</v>
@@ -3189,13 +3296,13 @@
     </row>
     <row r="12" spans="1:16" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -3204,25 +3311,25 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>157</v>
+        <v>312</v>
       </c>
       <c r="P12" t="b">
         <v>0</v>
@@ -3230,13 +3337,13 @@
     </row>
     <row r="13" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -3245,25 +3352,25 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>157</v>
+        <v>313</v>
       </c>
       <c r="P13" t="b">
         <v>0</v>
@@ -3271,13 +3378,13 @@
     </row>
     <row r="14" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -3286,25 +3393,25 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>157</v>
+        <v>314</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -3312,13 +3419,13 @@
     </row>
     <row r="15" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -3327,25 +3434,25 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>157</v>
+        <v>315</v>
       </c>
       <c r="P15" t="b">
         <v>0</v>
@@ -3353,13 +3460,13 @@
     </row>
     <row r="16" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -3368,25 +3475,25 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>157</v>
+        <v>316</v>
       </c>
       <c r="P16" t="b">
         <v>0</v>
@@ -3394,13 +3501,13 @@
     </row>
     <row r="17" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -3409,25 +3516,25 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>157</v>
+        <v>317</v>
       </c>
       <c r="P17" t="b">
         <v>0</v>
@@ -3435,13 +3542,13 @@
     </row>
     <row r="18" spans="1:16" ht="204" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -3450,25 +3557,25 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="P18" t="b">
         <v>0</v>
@@ -3497,39 +3604,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C1" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" t="s">
         <v>213</v>
-      </c>
-      <c r="C2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E2" t="s">
-        <v>232</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3537,19 +3644,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3557,19 +3664,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3577,19 +3684,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="E5" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3597,19 +3704,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="E6" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3617,19 +3724,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3637,19 +3744,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3657,19 +3764,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3677,19 +3784,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3697,19 +3804,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3748,476 +3855,476 @@
   <sheetData>
     <row r="1" spans="1:18" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="H1" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="K1" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="R1" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P2" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P3" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P4" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="B5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P5" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="B6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P6" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="B7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O7" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P7" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O8" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P8" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="B9" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O9" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P9" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="B10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P10" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="B11" t="s">
+        <v>257</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="O11" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="P11" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" t="s">
         <v>223</v>
-      </c>
-      <c r="B12" t="s">
-        <v>242</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -4255,10 +4362,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4296,10 +4403,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -4337,10 +4444,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -4378,10 +4485,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="B16" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -4419,10 +4526,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -4460,10 +4567,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -4501,10 +4608,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -4542,10 +4649,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4583,10 +4690,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -4632,8 +4739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7873D7B5-42F6-EA4D-BE3A-EF8367D067FD}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4645,19 +4752,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="E1" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4668,13 +4775,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>269</v>
+        <v>323</v>
       </c>
       <c r="E2" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4685,13 +4792,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>270</v>
+        <v>322</v>
       </c>
       <c r="E3" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4702,13 +4809,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="E4" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4719,13 +4826,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>272</v>
+        <v>325</v>
       </c>
       <c r="E5" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4736,13 +4843,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="E6" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4753,13 +4860,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4770,13 +4877,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4787,13 +4894,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="E9" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4804,13 +4911,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="E10" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -4821,13 +4928,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="E11" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -4896,19 +5003,19 @@
   <sheetData>
     <row r="1" spans="11:21" x14ac:dyDescent="0.2">
       <c r="L1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="M1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="N1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="O1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="Q1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="11:21" x14ac:dyDescent="0.2">
@@ -4991,7 +5098,7 @@
     </row>
     <row r="5" spans="11:21" x14ac:dyDescent="0.2">
       <c r="N5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="O5">
         <f>(P2+P3+P4) / 3</f>
@@ -5004,7 +5111,7 @@
     </row>
     <row r="7" spans="11:21" x14ac:dyDescent="0.2">
       <c r="N7" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O7">
         <f>O5/Q5</f>

</xml_diff>

<commit_message>
add item in task
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F525D1BF-614F-0C4F-9432-1B1915041F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCBB3E7-E95A-994F-BAED-2A018E516BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="454">
   <si>
     <t>ID</t>
   </si>
@@ -1581,6 +1581,14 @@
 item-24,10,false
 item-25,10,false
 item-26,10,false</t>
+  </si>
+  <si>
+    <t>Item
+itemid,quantity,당첨범위,전체범위</t>
+  </si>
+  <si>
+    <t>item-1,3,10,10
+item-2,1,50,100</t>
   </si>
 </sst>
 </file>
@@ -2455,10 +2463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2475,12 +2483,13 @@
     <col min="13" max="13" width="20.1640625" customWidth="1"/>
     <col min="15" max="15" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="4"/>
-    <col min="18" max="18" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="4"/>
+    <col min="19" max="19" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="136" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2529,17 +2538,20 @@
       <c r="P1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>109</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -2575,14 +2587,14 @@
       <c r="O2" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>102</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -2618,14 +2630,14 @@
       <c r="O3" t="s">
         <v>92</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4">
         <v>104</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2665,14 +2677,14 @@
       <c r="O4" t="s">
         <v>290</v>
       </c>
-      <c r="Q4" s="4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2712,14 +2724,14 @@
       <c r="O5" t="s">
         <v>291</v>
       </c>
-      <c r="Q5" s="4">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="4">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2759,14 +2771,17 @@
       <c r="O6" t="s">
         <v>292</v>
       </c>
-      <c r="Q6" s="4">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2806,14 +2821,14 @@
       <c r="O7" t="s">
         <v>293</v>
       </c>
-      <c r="Q7" s="4">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2853,14 +2868,14 @@
       <c r="O8" t="s">
         <v>294</v>
       </c>
-      <c r="Q8" s="4">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2900,14 +2915,14 @@
       <c r="O9" t="s">
         <v>295</v>
       </c>
-      <c r="Q9" s="4">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="R9" s="4">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2947,14 +2962,14 @@
       <c r="O10" t="s">
         <v>296</v>
       </c>
-      <c r="Q10" s="4">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="R10" s="4">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2994,14 +3009,14 @@
       <c r="O11" t="s">
         <v>297</v>
       </c>
-      <c r="Q11" s="4">
-        <v>1</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3041,14 +3056,14 @@
       <c r="O12" t="s">
         <v>298</v>
       </c>
-      <c r="Q12" s="4">
-        <v>1</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3091,14 +3106,14 @@
       <c r="O13" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="4">
-        <v>1</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="R13" s="4">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3133,14 +3148,14 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="Q14" s="4">
-        <v>1</v>
-      </c>
-      <c r="R14" t="s">
+      <c r="R14" s="4">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3183,14 +3198,14 @@
       <c r="O15" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="4">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="R15" s="4">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -3227,13 +3242,13 @@
       <c r="O16" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="4">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="R16" s="4">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
         <v>121</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3247,7 +3262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add L10n & market price
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C551C0-55B9-A44D-AB6A-49995CBA9877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6286418-67CC-AF46-A09B-2497FBD2E535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,12 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$V$2:$V$17</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$W$2:$W$17</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$V$2:$V$17</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$W$2:$W$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="489">
   <si>
     <t>ID</t>
   </si>
@@ -1006,42 +1012,6 @@
   </si>
   <si>
     <t>12,8,6</t>
-  </si>
-  <si>
-    <t>HP,27,50,8</t>
-  </si>
-  <si>
-    <t>MP,20,50,8</t>
-  </si>
-  <si>
-    <t>Gold,20,50,8</t>
-  </si>
-  <si>
-    <t>Ability1,20,50,0</t>
-  </si>
-  <si>
-    <t>Ability2,20,50,0</t>
-  </si>
-  <si>
-    <t>Ability3,20,50,0</t>
-  </si>
-  <si>
-    <t>Resource1,20,50,0</t>
-  </si>
-  <si>
-    <t>Resource2,20,50,0</t>
-  </si>
-  <si>
-    <t>Resource3,20,50,0</t>
-  </si>
-  <si>
-    <t>Sight,20,50,0</t>
-  </si>
-  <si>
-    <t>Leadership,0,50,0</t>
-  </si>
-  <si>
-    <t>Friendship,0,50,0</t>
   </si>
   <si>
     <t>6,8,12</t>
@@ -1622,13 +1592,6 @@
     <t>1.Satisfaction.Resource1:max</t>
   </si>
   <si>
-    <t>Resource1:1,Gold:$|-10|%</t>
-  </si>
-  <si>
-    <t>satisfactions
-$|-10|%: 시세보다 10% 저렴한 비용</t>
-  </si>
-  <si>
     <t>자원1 $|-10|% 골드에 쿨거래 가능?</t>
   </si>
   <si>
@@ -1637,6 +1600,23 @@
   </si>
   <si>
     <t>좋아 우리 친하잖아</t>
+  </si>
+  <si>
+    <t>수요곡선</t>
+  </si>
+  <si>
+    <t>기울기</t>
+  </si>
+  <si>
+    <t>절편</t>
+  </si>
+  <si>
+    <t>Resource1:1,Gold:$|0.9|-%</t>
+  </si>
+  <si>
+    <t>satisfactions
+$|0.9|-%: 시세보다 10% 저렴한 비용 차감
+$|1.1|+%: 시세보다 10% 비싼 비용 획득</t>
   </si>
 </sst>
 </file>
@@ -2211,6 +2191,1008 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0" i="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>demand curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$V$2:$V$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$2:$W$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0AE9-A54E-857E-AED173DC1112}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2140522096"/>
+        <c:axId val="970109215"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2140522096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="970109215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="970109215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140522096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF718A4-DEB4-7D2F-0324-33DC6E1F6624}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2510,8 +3492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2578,13 +3560,13 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>124</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>13</v>
@@ -2696,10 +3678,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -2726,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -2743,13 +3725,13 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="H5" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2761,7 +3743,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -2773,12 +3755,12 @@
         <v>1</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -2790,13 +3772,13 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="H6" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -2808,19 +3790,19 @@
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="R6" s="4">
         <v>1</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -2843,7 +3825,7 @@
         <v>274</v>
       </c>
       <c r="H7" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2855,7 +3837,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2868,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -2935,7 +3917,7 @@
         <v>276</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -2982,7 +3964,7 @@
         <v>277</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H10" t="s">
         <v>17</v>
@@ -3026,13 +4008,13 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="H11" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -3050,10 +4032,10 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="R11" s="4">
         <v>1</v>
@@ -3076,13 +4058,13 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="H12" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -3100,10 +4082,10 @@
         <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="R12" s="4">
         <v>1</v>
@@ -3126,13 +4108,13 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="H13" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -3150,10 +4132,10 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="R13" s="4">
         <v>1</v>
@@ -3353,10 +4335,10 @@
     </row>
     <row r="18" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="B18" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -3368,10 +4350,10 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>
@@ -3386,27 +4368,27 @@
         <v>2</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="Q18" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="R18" s="4">
         <v>1</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3418,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="H19" t="s">
         <v>17</v>
@@ -3433,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -3442,12 +4424,12 @@
         <v>1</v>
       </c>
       <c r="S19" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3459,10 +4441,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="H20" t="s">
         <v>33</v>
@@ -3477,27 +4459,27 @@
         <v>3</v>
       </c>
       <c r="L20" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="M20">
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="O20" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="R20" s="4">
         <v>1</v>
       </c>
       <c r="S20" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3536,10 +4518,10 @@
         <v>1</v>
       </c>
       <c r="S21" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -3552,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3612,13 +4594,13 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="P1" t="s">
         <v>107</v>
       </c>
       <c r="Q1" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="34" x14ac:dyDescent="0.2">
@@ -3770,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>63</v>
@@ -3922,7 +4904,7 @@
     </row>
     <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3934,16 +4916,16 @@
         <v>108</v>
       </c>
       <c r="F9" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>95</v>
@@ -3955,7 +4937,7 @@
         <v>15</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="P9" t="b">
         <v>0</v>
@@ -4025,7 +5007,7 @@
         <v>93</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
         <v>94</v>
@@ -4040,10 +5022,10 @@
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="P11" t="b">
         <v>0</v>
@@ -4087,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P12" t="b">
         <v>0</v>
@@ -4131,7 +5113,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P13" t="b">
         <v>0</v>
@@ -4175,7 +5157,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -4219,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P15" t="b">
         <v>0</v>
@@ -4263,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P16" t="b">
         <v>0</v>
@@ -4307,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P17" t="b">
         <v>0</v>
@@ -4351,7 +5333,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="P18" t="b">
         <v>0</v>
@@ -5554,16 +6536,16 @@
     </row>
     <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="B22" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="C22" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D22" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -5578,7 +6560,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="L22" s="7">
         <v>0</v>
@@ -5601,16 +6583,16 @@
     </row>
     <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="B23" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="C23" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="D23" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -5625,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="L23" s="7">
         <v>0</v>
@@ -5648,16 +6630,16 @@
     </row>
     <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B24" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="C24" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="D24" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -5672,7 +6654,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="L24" s="7">
         <v>0</v>
@@ -5695,19 +6677,19 @@
     </row>
     <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="B25" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="C25" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="D25" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="E25" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -5716,7 +6698,7 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -5725,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="L25" s="7">
         <v>12</v>
@@ -5748,19 +6730,19 @@
     </row>
     <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B26" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="C26" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E26" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -5798,19 +6780,19 @@
     </row>
     <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B27" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="C27" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D27" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E27" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -5848,19 +6830,19 @@
     </row>
     <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="B28" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="C28" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D28" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E28" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -5898,19 +6880,19 @@
     </row>
     <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="B29" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="C29" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D29" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E29" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -5948,19 +6930,19 @@
     </row>
     <row r="30" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="B30" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="C30" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D30" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E30" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -5998,19 +6980,19 @@
     </row>
     <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B31" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C31" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D31" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E31" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -6048,19 +7030,19 @@
     </row>
     <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B32" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="C32" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D32" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E32" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -6098,19 +7080,19 @@
     </row>
     <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B33" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="C33" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D33" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E33" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -6148,19 +7130,19 @@
     </row>
     <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B34" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="C34" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D34" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E34" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -6198,19 +7180,19 @@
     </row>
     <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="B35" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="C35" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D35" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E35" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -6248,19 +7230,19 @@
     </row>
     <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="B36" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="C36" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D36" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E36" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -6298,19 +7280,19 @@
     </row>
     <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="B37" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="C37" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D37" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E37" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -6348,19 +7330,19 @@
     </row>
     <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="B38" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="C38" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D38" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E38" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -6398,19 +7380,19 @@
     </row>
     <row r="39" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="B39" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="C39" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D39" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E39" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -6448,19 +7430,19 @@
     </row>
     <row r="40" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="B40" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="C40" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D40" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E40" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -6498,19 +7480,19 @@
     </row>
     <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="B41" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="C41" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D41" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E41" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -6548,19 +7530,19 @@
     </row>
     <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="B42" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="C42" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D42" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E42" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -6598,19 +7580,19 @@
     </row>
     <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="B43" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="C43" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D43" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E43" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -6648,19 +7630,19 @@
     </row>
     <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="B44" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C44" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D44" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E44" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -6698,19 +7680,19 @@
     </row>
     <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="B45" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C45" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D45" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E45" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -6748,19 +7730,19 @@
     </row>
     <row r="46" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="B46" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="C46" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D46" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E46" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -6798,19 +7780,19 @@
     </row>
     <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B47" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="C47" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D47" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E47" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -6848,19 +7830,19 @@
     </row>
     <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="B48" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="C48" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D48" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E48" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -6898,19 +7880,19 @@
     </row>
     <row r="49" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="B49" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="C49" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D49" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E49" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -6948,19 +7930,19 @@
     </row>
     <row r="50" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="B50" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="C50" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D50" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E50" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -6998,19 +7980,19 @@
     </row>
     <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="B51" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="C51" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D51" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E51" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -7048,19 +8030,19 @@
     </row>
     <row r="52" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B52" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="C52" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D52" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E52" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -7098,19 +8080,19 @@
     </row>
     <row r="53" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="B53" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="C53" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D53" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E53" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -7148,19 +8130,19 @@
     </row>
     <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="B54" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="C54" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D54" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E54" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -7198,19 +8180,19 @@
     </row>
     <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="B55" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="C55" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D55" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E55" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -7248,19 +8230,19 @@
     </row>
     <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B56" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="C56" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D56" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E56" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -7298,19 +8280,19 @@
     </row>
     <row r="57" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="B57" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="C57" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D57" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E57" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -7348,19 +8330,19 @@
     </row>
     <row r="58" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="B58" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="C58" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D58" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E58" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -7398,19 +8380,19 @@
     </row>
     <row r="59" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B59" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="C59" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D59" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E59" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -7710,15 +8692,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511382C-D11B-5A44-B5FF-0A23CC8CA529}">
-  <dimension ref="K1:R37"/>
+  <dimension ref="K1:Z36"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="11:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="11:26" x14ac:dyDescent="0.2">
       <c r="L1" t="s">
         <v>146</v>
       </c>
@@ -7734,8 +8716,17 @@
       <c r="Q1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="W1" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="11:26" x14ac:dyDescent="0.2">
       <c r="K2" t="s">
         <v>16</v>
       </c>
@@ -7760,8 +8751,21 @@
         <f>POWER(P2-O5,2)</f>
         <v>4.9382716049382858E-4</v>
       </c>
-    </row>
-    <row r="3" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <f>Y2*V2+Z2</f>
+        <v>35</v>
+      </c>
+      <c r="Y2">
+        <v>-2</v>
+      </c>
+      <c r="Z2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="11:26" x14ac:dyDescent="0.2">
       <c r="K3" t="s">
         <v>19</v>
       </c>
@@ -7786,8 +8790,15 @@
         <f>POWER(P3-O5,2)</f>
         <v>1.49382716049383E-2</v>
       </c>
-    </row>
-    <row r="4" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <f>Y2*V3+Z2</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="11:26" x14ac:dyDescent="0.2">
       <c r="K4" t="s">
         <v>21</v>
       </c>
@@ -7812,8 +8823,15 @@
         <f>POWER(P4-O5,2)</f>
         <v>2.0864197530864177E-2</v>
       </c>
-    </row>
-    <row r="5" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <f>Y2*V4+Z2</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="11:26" x14ac:dyDescent="0.2">
       <c r="N5" t="s">
         <v>144</v>
       </c>
@@ -7828,8 +8846,24 @@
         <f>SQRT((Q2+Q3+Q4) /3)</f>
         <v>0.10999438818457408</v>
       </c>
-    </row>
-    <row r="7" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <f>Y2*V5+Z2</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <f>Y2*V6+Z2</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="11:26" x14ac:dyDescent="0.2">
       <c r="N7" t="s">
         <v>150</v>
       </c>
@@ -7837,101 +8871,137 @@
         <f>O5/POWER(Q5,2)</f>
         <v>-56.02040816326528</v>
       </c>
-    </row>
-    <row r="8" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V7">
+        <v>6</v>
+      </c>
+      <c r="W7">
+        <f>Y2*V7+Z2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="11:26" x14ac:dyDescent="0.2">
       <c r="Q8" t="s">
         <v>144</v>
       </c>
       <c r="R8" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="9" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V8">
+        <v>7</v>
+      </c>
+      <c r="W8">
+        <f>Y2*V8+Z2</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="11:26" x14ac:dyDescent="0.2">
       <c r="P9" t="s">
         <v>300</v>
       </c>
       <c r="Q9">
         <v>-0.73299999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V9">
+        <v>8</v>
+      </c>
+      <c r="W9">
+        <f>Y2*V9+Z2</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="11:26" x14ac:dyDescent="0.2">
       <c r="P10" t="s">
         <v>301</v>
       </c>
       <c r="Q10">
         <v>-0.71099999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="11:18" x14ac:dyDescent="0.2">
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="W10">
+        <f>Y2*V10+Z2</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="11:26" x14ac:dyDescent="0.2">
       <c r="P11" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="Q11">
         <v>-0.67700000000000005</v>
       </c>
-    </row>
-    <row r="26" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K26" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="27" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K27" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K28" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="29" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K29" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="30" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K30" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="31" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K31" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="32" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K32" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K33" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K34" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K35" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K36" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K37" t="s">
-        <v>313</v>
+      <c r="V11">
+        <v>10</v>
+      </c>
+      <c r="W11">
+        <f>Y2*V11+Z2</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="V12">
+        <v>11</v>
+      </c>
+      <c r="W12">
+        <f>Y2*V12+Z2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="V13">
+        <v>12</v>
+      </c>
+      <c r="W13">
+        <f>Y2*V13+Z2</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="V14">
+        <v>13</v>
+      </c>
+      <c r="W14">
+        <f>Y2*V14+Z2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="V15">
+        <v>14</v>
+      </c>
+      <c r="W15">
+        <f>Y2*V15+Z2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="V16">
+        <v>15</v>
+      </c>
+      <c r="W16">
+        <f>Y2*V16+Z2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="22:23" x14ac:dyDescent="0.2">
+      <c r="V17">
+        <v>16</v>
+      </c>
+      <c r="W17">
+        <f>Y2*V17+Z2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T36">
+        <f>-2*58+512</f>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7952,164 +9022,164 @@
   <sheetData>
     <row r="2" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="J2" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="J3" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I4" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I5" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="J5" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="J6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I7" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="J7" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="J8" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I9" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="J9" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="J10" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="J11" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
+        <v>322</v>
+      </c>
+      <c r="J12" t="s">
         <v>334</v>
-      </c>
-      <c r="J12" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="13" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="J13" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="J15" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="J16" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="J17" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I18" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="J18" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="K18" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="J19" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="J20" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="J21" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add pool, singleton, stock config and more
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A4162-6ED4-F743-BB62-8755410189B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4BC53A-2905-6B45-8CB4-BB36EAD4BF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="705">
   <si>
     <t>ID</t>
   </si>
@@ -2291,7 +2291,10 @@
     <t>친근감</t>
   </si>
   <si>
-    <t>Gold,0,0,148
+    <t>stock market default price</t>
+  </si>
+  <si>
+    <t>Gold,0,0,3.5
 Speed,1,4,2
 HP,20,50,8
 MP,20,50,15
@@ -2299,7 +2302,7 @@
 Ability1,20,50,0
 Ability2,20,50,0
 Ability3,20,50,0
-Resource1,20,50,40
+Resource1,20,50,5
 Resource2,20,50,40
 Resource3,20,50,40
 Sight,20,50,0
@@ -6019,7 +6022,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>655</v>
@@ -9752,10 +9755,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511382C-D11B-5A44-B5FF-0A23CC8CA529}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9763,11 +9766,12 @@
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -9783,8 +9787,11 @@
       <c r="E1" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -9801,7 +9808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>684</v>
       </c>
@@ -9818,7 +9825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -9835,7 +9842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -9852,7 +9859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>688</v>
       </c>
@@ -9869,7 +9876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>690</v>
       </c>
@@ -9886,7 +9893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>692</v>
       </c>
@@ -9903,7 +9910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>694</v>
       </c>
@@ -9920,7 +9927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>697</v>
       </c>
@@ -9937,7 +9944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>699</v>
       </c>
@@ -9954,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>701</v>
       </c>
@@ -9971,7 +9978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>385</v>
       </c>
@@ -9987,8 +9994,11 @@
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>390</v>
       </c>
@@ -10004,8 +10014,11 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>391</v>
       </c>
@@ -10020,6 +10033,9 @@
       </c>
       <c r="E15">
         <v>0</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add l10n code gen
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761E3332-D9FF-584E-AFC0-561918839C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1F043-1A4C-8E45-8564-2F071B196382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task" sheetId="1" r:id="rId1"/>
     <sheet name="actors" sheetId="2" r:id="rId2"/>
     <sheet name="quest" sheetId="4" r:id="rId3"/>
     <sheet name="item" sheetId="5" r:id="rId4"/>
-    <sheet name="level" sheetId="6" r:id="rId5"/>
-    <sheet name="vehicle" sheetId="8" r:id="rId6"/>
-    <sheet name="satisfaction" sheetId="3" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId8"/>
+    <sheet name="l10n" sheetId="9" r:id="rId5"/>
+    <sheet name="level" sheetId="6" r:id="rId6"/>
+    <sheet name="vehicle" sheetId="8" r:id="rId7"/>
+    <sheet name="satisfaction" sheetId="3" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="729">
   <si>
     <t>ID</t>
   </si>
@@ -2317,6 +2318,69 @@
   </si>
   <si>
     <t>자원 시장에서 거래를 할 수도 요리의 재료로 사용할 수도 있다</t>
+  </si>
+  <si>
+    <t>오예! 레벨업!</t>
+  </si>
+  <si>
+    <t>세금 징수</t>
+  </si>
+  <si>
+    <t>이동 거리가 너무 가까워 탑승에 실패 했습니다</t>
+  </si>
+  <si>
+    <t>거래소에 등록한 자원이 판매 되었습니다</t>
+  </si>
+  <si>
+    <t>거래소에 등록한 자원이 구매 되었습니다</t>
+  </si>
+  <si>
+    <t>STOCK_BUY</t>
+  </si>
+  <si>
+    <t>자원</t>
+  </si>
+  <si>
+    <t>UI_INVEN_TAP_RESOURCE</t>
+  </si>
+  <si>
+    <t>장착템</t>
+  </si>
+  <si>
+    <t>버리기</t>
+  </si>
+  <si>
+    <t>사용</t>
+  </si>
+  <si>
+    <t>LEVEL_UP</t>
+  </si>
+  <si>
+    <t>TAX_COLLECTION</t>
+  </si>
+  <si>
+    <t>GET_IN_VEHICLE_FAILURE</t>
+  </si>
+  <si>
+    <t>STOCK_SELL</t>
+  </si>
+  <si>
+    <t>UI_INVEN_TAP_ITEM</t>
+  </si>
+  <si>
+    <t>UI_INVEN_TAP_INSTALLATION</t>
+  </si>
+  <si>
+    <t>UI_INVEN_USE</t>
+  </si>
+  <si>
+    <t>UI_INVEN_ABANDON</t>
+  </si>
+  <si>
+    <t>UI_INVEN_BUY</t>
+  </si>
+  <si>
+    <t>구매</t>
   </si>
 </sst>
 </file>
@@ -9356,6 +9420,113 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F8AB1-4340-124F-87D9-2427FE940228}">
+  <dimension ref="A2:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>719</v>
+      </c>
+      <c r="B2" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>720</v>
+      </c>
+      <c r="B3" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>721</v>
+      </c>
+      <c r="B4" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B5" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>713</v>
+      </c>
+      <c r="B6" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>723</v>
+      </c>
+      <c r="B7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>715</v>
+      </c>
+      <c r="B8" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>724</v>
+      </c>
+      <c r="B9" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>725</v>
+      </c>
+      <c r="B10" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>726</v>
+      </c>
+      <c r="B11" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>727</v>
+      </c>
+      <c r="B12" t="s">
+        <v>728</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7873D7B5-42F6-EA4D-BE3A-EF8367D067FD}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9611,7 +9782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920B6BC8-09F3-3245-B8D8-73897C533FE3}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -9762,11 +9933,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511382C-D11B-5A44-B5FF-0A23CC8CA529}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -10065,7 +10236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404C2200-8081-644A-AB13-9EC51CCA238B}">
   <dimension ref="A2:N46"/>
   <sheetViews>

</xml_diff>

<commit_message>
add ask title, desc
</commit_message>
<xml_diff>
--- a/config_gen/config.xlsx
+++ b/config_gen/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daejung/work/unity/Lemmings/Assets/Script/AI/config_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB2A88D-643D-EB4C-A458-2A13282F63DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A85F4F-F0AB-5D40-80C3-C9B0C2167A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="773">
   <si>
     <t>ID</t>
   </si>
@@ -2507,6 +2507,21 @@
   </si>
   <si>
     <t>이동!</t>
+  </si>
+  <si>
+    <t>Ask Desc</t>
+  </si>
+  <si>
+    <t>Ask Title</t>
+  </si>
+  <si>
+    <t>{from}이/가 주제도 모르고 감히 인사를 하겠다고 합니다.
+아마도 돈을 노리고 저러는거 같은데 수락하시겠습니까?
+수락할 경우 MP +5
+거절할 경우 김밥이는 MP -10이 됩니다.</t>
+  </si>
+  <si>
+    <t>괜히 친한척 하며 말을 걸어 왔습니다.</t>
   </si>
 </sst>
 </file>
@@ -3397,11 +3412,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X53"/>
+  <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W35" sqref="W35"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3426,9 +3441,11 @@
     <col min="21" max="21" width="36.83203125" customWidth="1"/>
     <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="187" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="187" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3501,8 +3518,14 @@
       <c r="X1" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y1" t="s">
+        <v>770</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -3548,7 +3571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3594,7 +3617,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>491</v>
       </c>
@@ -3642,7 +3665,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3692,7 +3715,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3742,7 +3765,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>407</v>
       </c>
@@ -3792,7 +3815,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -3845,7 +3868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>443</v>
       </c>
@@ -3897,7 +3920,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -3947,7 +3970,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3997,7 +4020,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4047,7 +4070,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4101,7 +4124,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -4155,7 +4178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -4209,7 +4232,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -4262,7 +4285,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -4307,7 +4330,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -4359,8 +4382,14 @@
       <c r="V18" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="Y18" t="s">
+        <v>772</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -4410,7 +4439,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>414</v>
       </c>
@@ -4466,7 +4495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>429</v>
       </c>
@@ -4510,7 +4539,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>433</v>
       </c>
@@ -4563,7 +4592,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>434</v>
       </c>
@@ -4613,7 +4642,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>469</v>
       </c>
@@ -4666,7 +4695,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>467</v>
       </c>
@@ -4707,7 +4736,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>453</v>
       </c>
@@ -4745,7 +4774,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>470</v>
       </c>
@@ -4798,7 +4827,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>471</v>
       </c>
@@ -4839,7 +4868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>497</v>
       </c>
@@ -4895,7 +4924,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>501</v>
       </c>
@@ -4942,7 +4971,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>510</v>
       </c>
@@ -4995,7 +5024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>511</v>
       </c>

</xml_diff>